<commit_message>
updating README with up to date API calls.  Adding amphibianDisease instructions
</commit_message>
<xml_diff>
--- a/amphibianDisease/amphibianDisease.xlsx
+++ b/amphibianDisease/amphibianDisease.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdeck/IdeaProjects/geome-configurations/amphibianDisease/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AE1E43-3718-2341-AF78-BEDC63E68A81}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68AFE70-0298-4649-AE1A-E8059D6EB867}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5980" yWindow="4060" windowWidth="27240" windowHeight="16440" xr2:uid="{EE213A37-7B2B-0548-A624-8FB513D29C9B}"/>
+    <workbookView xWindow="2760" yWindow="460" windowWidth="13840" windowHeight="17540" xr2:uid="{EE213A37-7B2B-0548-A624-8FB513D29C9B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Samples" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="99">
   <si>
     <t>sampleID</t>
   </si>
@@ -69,9 +69,6 @@
     <t>sampleType</t>
   </si>
   <si>
-    <t>preparationType</t>
-  </si>
-  <si>
     <t>specimenDisposition</t>
   </si>
   <si>
@@ -273,9 +270,6 @@
     <t>Number of zoospore detected. Needed to calculate Zoospore Equivalent Score (ZEscore), a measure of infection intensity (see Vredenburg et al 2010 doi: 10.1073/pnas.0914111107)</t>
   </si>
   <si>
-    <t>sampleType (see sampleType field) dilution factor. Needed to calculate Zoospore Equivalent Score (ZEscore), a measure of infection intensity (see Vredenburg et al 2010 doi: 10.1073/pnas.0914111107)</t>
-  </si>
-  <si>
     <t>Cycle number ("c(t)") at which the qPCR machine first detects a positive for chytrid ( a measure of the amount of Bd or Bsal present)</t>
   </si>
   <si>
@@ -285,13 +279,55 @@
     <t>If present, these values may be entered (otherwise it will be calculated from the quantityDetected and dilutionFactor).</t>
   </si>
   <si>
-    <t>TRUE, FALSE</t>
-  </si>
-  <si>
     <t>fasta?</t>
   </si>
   <si>
     <t>principalInvestigator</t>
+  </si>
+  <si>
+    <t>diseaseDetected</t>
+  </si>
+  <si>
+    <t>quantityDected</t>
+  </si>
+  <si>
+    <t>testMethod</t>
+  </si>
+  <si>
+    <t>diseaseSampling</t>
+  </si>
+  <si>
+    <t>zeScore</t>
+  </si>
+  <si>
+    <t>column</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>uri</t>
+  </si>
+  <si>
+    <t>dataType</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>Type of sample tested: eg, swabbing, blood, skin, liver</t>
+  </si>
+  <si>
+    <t>Post-sampling status</t>
+  </si>
+  <si>
+    <t>The dilution factor is needed to calculate Zoospore Equivalent Score (ZEscore), a measure of infection intensity (see Vredenburg et al 2010 doi: 10.1073/pnas.0914111107)</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>"internal": false, "allowUnknown": false, "allowTBD": false</t>
   </si>
 </sst>
 </file>
@@ -321,12 +357,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -341,10 +389,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,504 +711,1083 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9974B0-4F07-3F40-862F-7C3240289FB3}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" customWidth="1"/>
-    <col min="4" max="5" width="49.33203125" customWidth="1"/>
-    <col min="6" max="6" width="64.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="49.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" customWidth="1"/>
+    <col min="8" max="8" width="49.33203125" customWidth="1"/>
+    <col min="9" max="9" width="64.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="G4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>39</v>
       </c>
-      <c r="C5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="G6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>27</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>40</v>
       </c>
-      <c r="C6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="G7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>28</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="G9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>30</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="G10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>31</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
         <v>43</v>
       </c>
-      <c r="C10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="G14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>35</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>44</v>
       </c>
-      <c r="C14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="G16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
         <v>52</v>
       </c>
-      <c r="B17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>0</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
       </c>
-      <c r="C18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>1</v>
       </c>
-      <c r="C19" t="s">
-        <v>73</v>
-      </c>
-      <c r="F19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>3</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
       </c>
-      <c r="C20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
       <c r="B21" t="s">
         <v>4</v>
       </c>
-      <c r="C21" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>5</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
       </c>
-      <c r="C22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
       </c>
-      <c r="C23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" t="s">
-        <v>73</v>
-      </c>
-      <c r="E24" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="G25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>17</v>
       </c>
       <c r="B26" t="s">
         <v>17</v>
       </c>
-      <c r="C26" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>18</v>
       </c>
       <c r="B27" t="s">
         <v>18</v>
       </c>
-      <c r="C27" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>19</v>
       </c>
       <c r="B28" t="s">
         <v>19</v>
       </c>
-      <c r="C28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="G29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" t="s">
+        <v>72</v>
+      </c>
+      <c r="H30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>20</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>20</v>
       </c>
-      <c r="C29" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="G31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" t="s">
+        <v>91</v>
+      </c>
+      <c r="E32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" t="s">
+        <v>75</v>
+      </c>
+      <c r="H32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="3" t="str">
+        <f>_xlfn.CONCAT("urn:",B33)</f>
+        <v>urn:sampleType</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" s="3" t="str">
+        <f>_xlfn.CONCAT("urn:",B34)</f>
+        <v>urn:diseaseLineage</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="B35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" s="3" t="str">
+        <f t="shared" ref="D35:D45" si="0">_xlfn.CONCAT("urn:",B35)</f>
+        <v>urn:genotypeMethod</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:diseaseTested</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:specimenDisposition</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:diseaseDetected</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H38" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:fatal</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" t="s">
-        <v>63</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" t="s">
-        <v>73</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="H39" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="17" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>15</v>
-      </c>
-      <c r="D36" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:testMethod</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F40" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="1" t="s">
+    </row>
+    <row r="41" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:quantityDected</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>16</v>
-      </c>
-      <c r="D37" t="s">
-        <v>84</v>
-      </c>
-      <c r="E37" s="1" t="s">
+    <row r="42" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D42" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:dilutionFactor</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:cycleTimeFirstDetection</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D44" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:diagnosticLab</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D45" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>urn:zeScore</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>37</v>
-      </c>
-      <c r="D38" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="17" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>47</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="17" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>48</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="17" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>49</v>
-      </c>
-      <c r="D42" s="1" t="s">
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" t="s">
+        <v>70</v>
+      </c>
+      <c r="G47" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="17" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>51</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>70</v>
-      </c>
-      <c r="C45" t="s">
-        <v>85</v>
-      </c>
-      <c r="E45" t="s">
-        <v>71</v>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B50" t="str">
+        <f>_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B33,CHAR(34))</f>
+        <v>"column":"sampleType"</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" ref="C50:F50" si="1">_xlfn.CONCAT(CHAR(34),C$32,CHAR(34),":",CHAR(34),C33,CHAR(34))</f>
+        <v>"group":"diseaseSampling"</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="1"/>
+        <v>"uri":"urn:sampleType"</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="1"/>
+        <v>"dataType":"String"</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="1"/>
+        <v>"definition":"Type of sample tested: eg, swabbing, blood, skin, liver"</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B51" t="str">
+        <f t="shared" ref="B51:F51" si="2">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B34,CHAR(34))</f>
+        <v>"column":"diseaseLineage"</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="2"/>
+        <v>"group":"diseaseSampling"</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="2"/>
+        <v>"uri":"urn:diseaseLineage"</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="2"/>
+        <v>"dataType":"String"</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" si="2"/>
+        <v>"definition":"Specific genetic lineage detected (if available) NCBI URI (e.g., http://www.ncbi.nlm.nih.gov/biosample/xxxxxxx"</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B52" t="str">
+        <f t="shared" ref="B52:F52" si="3">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B35,CHAR(34))</f>
+        <v>"column":"genotypeMethod"</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="3"/>
+        <v>"group":"diseaseSampling"</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="3"/>
+        <v>"uri":"urn:genotypeMethod"</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="3"/>
+        <v>"dataType":"String"</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="3"/>
+        <v>"definition":"Genotyping methods used to determine diseaseLineage if present (e.g., whole genome sequencing, ITS sequencing, multilocus nuclear sequencing)."</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B53" t="str">
+        <f t="shared" ref="B53:F53" si="4">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B36,CHAR(34))</f>
+        <v>"column":"diseaseTested"</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="4"/>
+        <v>"group":"diseaseSampling"</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="4"/>
+        <v>"uri":"urn:diseaseTested"</v>
+      </c>
+      <c r="E53" t="str">
+        <f t="shared" si="4"/>
+        <v>"dataType":"String"</v>
+      </c>
+      <c r="F53" t="str">
+        <f t="shared" si="4"/>
+        <v>"definition":"Controlled vocabulary: Bd, Bsal, Bd+Bsal, Other"</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B54" t="str">
+        <f t="shared" ref="B54:F54" si="5">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B37,CHAR(34))</f>
+        <v>"column":"specimenDisposition"</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="5"/>
+        <v>"group":"diseaseSampling"</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="5"/>
+        <v>"uri":"urn:specimenDisposition"</v>
+      </c>
+      <c r="E54" t="str">
+        <f t="shared" si="5"/>
+        <v>"dataType":"String"</v>
+      </c>
+      <c r="F54" t="str">
+        <f t="shared" si="5"/>
+        <v>"definition":"Post-sampling status"</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B55" t="str">
+        <f t="shared" ref="B55:F55" si="6">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B38,CHAR(34))</f>
+        <v>"column":"diseaseDetected"</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="6"/>
+        <v>"group":"diseaseSampling"</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="6"/>
+        <v>"uri":"urn:diseaseDetected"</v>
+      </c>
+      <c r="E55" t="str">
+        <f t="shared" si="6"/>
+        <v>"dataType":"String"</v>
+      </c>
+      <c r="F55" t="str">
+        <f t="shared" si="6"/>
+        <v>"definition":"Result of disease testing: True=Positive, False=Negative, No Confidence=Ambiguous"</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B56" t="str">
+        <f t="shared" ref="B56:F56" si="7">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B39,CHAR(34))</f>
+        <v>"column":"fatal"</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="7"/>
+        <v>"group":"diseaseSampling"</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="7"/>
+        <v>"uri":"urn:fatal"</v>
+      </c>
+      <c r="E56" t="str">
+        <f t="shared" si="7"/>
+        <v>"dataType":"String"</v>
+      </c>
+      <c r="F56" t="str">
+        <f t="shared" si="7"/>
+        <v>"definition":"At time of sampling, presumed cause of death to be diseaseTested, mark [FALSE] if unknown"</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B57" t="str">
+        <f t="shared" ref="B57:F57" si="8">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B40,CHAR(34))</f>
+        <v>"column":"testMethod"</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="8"/>
+        <v>"group":"diseaseSampling"</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="8"/>
+        <v>"uri":"urn:testMethod"</v>
+      </c>
+      <c r="E57" t="str">
+        <f t="shared" si="8"/>
+        <v>"dataType":"String"</v>
+      </c>
+      <c r="F57" t="str">
+        <f t="shared" si="8"/>
+        <v>"definition":"traditional PCR, quantitive PCR, realtime PCR, histology, Other"</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B58" t="str">
+        <f t="shared" ref="B58:F58" si="9">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B41,CHAR(34))</f>
+        <v>"column":"quantityDected"</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="9"/>
+        <v>"group":"diseaseSampling"</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="9"/>
+        <v>"uri":"urn:quantityDected"</v>
+      </c>
+      <c r="E58" t="str">
+        <f t="shared" si="9"/>
+        <v>"dataType":"String"</v>
+      </c>
+      <c r="F58" t="str">
+        <f t="shared" si="9"/>
+        <v>"definition":"Number of zoospore detected. Needed to calculate Zoospore Equivalent Score (ZEscore), a measure of infection intensity (see Vredenburg et al 2010 doi: 10.1073/pnas.0914111107)"</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B59" t="str">
+        <f t="shared" ref="B59:F59" si="10">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B42,CHAR(34))</f>
+        <v>"column":"dilutionFactor"</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="10"/>
+        <v>"group":"diseaseSampling"</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="10"/>
+        <v>"uri":"urn:dilutionFactor"</v>
+      </c>
+      <c r="E59" t="str">
+        <f t="shared" si="10"/>
+        <v>"dataType":"String"</v>
+      </c>
+      <c r="F59" t="str">
+        <f t="shared" si="10"/>
+        <v>"definition":"The dilution factor is needed to calculate Zoospore Equivalent Score (ZEscore), a measure of infection intensity (see Vredenburg et al 2010 doi: 10.1073/pnas.0914111107)"</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B60" t="str">
+        <f t="shared" ref="B60:F60" si="11">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B43,CHAR(34))</f>
+        <v>"column":"cycleTimeFirstDetection"</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="11"/>
+        <v>"group":"diseaseSampling"</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="11"/>
+        <v>"uri":"urn:cycleTimeFirstDetection"</v>
+      </c>
+      <c r="E60" t="str">
+        <f t="shared" si="11"/>
+        <v>"dataType":"String"</v>
+      </c>
+      <c r="F60" t="str">
+        <f t="shared" si="11"/>
+        <v>"definition":"Cycle number ("c(t)") at which the qPCR machine first detects a positive for chytrid ( a measure of the amount of Bd or Bsal present)"</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B61" t="str">
+        <f t="shared" ref="B61:F61" si="12">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B44,CHAR(34))</f>
+        <v>"column":"diagnosticLab"</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="12"/>
+        <v>"group":"diseaseSampling"</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="12"/>
+        <v>"uri":"urn:diagnosticLab"</v>
+      </c>
+      <c r="E61" t="str">
+        <f t="shared" si="12"/>
+        <v>"dataType":"String"</v>
+      </c>
+      <c r="F61" t="str">
+        <f t="shared" si="12"/>
+        <v>"definition":"Record the diagnostic lab if different than the diagnostic lab listed in the Project details or if more than one are used."</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B62" t="str">
+        <f t="shared" ref="B62:F62" si="13">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B45,CHAR(34))</f>
+        <v>"column":"zeScore"</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="13"/>
+        <v>"group":"diseaseSampling"</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="13"/>
+        <v>"uri":"urn:zeScore"</v>
+      </c>
+      <c r="E62" t="str">
+        <f t="shared" si="13"/>
+        <v>"dataType":"String"</v>
+      </c>
+      <c r="F62" t="str">
+        <f t="shared" si="13"/>
+        <v>"definition":"If present, these values may be entered (otherwise it will be calculated from the quantityDetected and dilutionFactor)."</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B64" t="str">
+        <f>_xlfn.CONCAT("{",B50,",",C50,",",D50,",",E50,",",F50,",",$A$63,"}")</f>
+        <v>{"column":"sampleType","group":"diseaseSampling","uri":"urn:sampleType","dataType":"String","definition":"Type of sample tested: eg, swabbing, blood, skin, liver","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B65" t="str">
+        <f t="shared" ref="B65:B76" si="14">_xlfn.CONCAT("{",B51,",",C51,",",D51,",",E51,",",F51,",",$A$63,"}")</f>
+        <v>{"column":"diseaseLineage","group":"diseaseSampling","uri":"urn:diseaseLineage","dataType":"String","definition":"Specific genetic lineage detected (if available) NCBI URI (e.g., http://www.ncbi.nlm.nih.gov/biosample/xxxxxxx","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B66" t="str">
+        <f t="shared" si="14"/>
+        <v>{"column":"genotypeMethod","group":"diseaseSampling","uri":"urn:genotypeMethod","dataType":"String","definition":"Genotyping methods used to determine diseaseLineage if present (e.g., whole genome sequencing, ITS sequencing, multilocus nuclear sequencing).","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B67" t="str">
+        <f t="shared" si="14"/>
+        <v>{"column":"diseaseTested","group":"diseaseSampling","uri":"urn:diseaseTested","dataType":"String","definition":"Controlled vocabulary: Bd, Bsal, Bd+Bsal, Other","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B68" t="str">
+        <f t="shared" si="14"/>
+        <v>{"column":"specimenDisposition","group":"diseaseSampling","uri":"urn:specimenDisposition","dataType":"String","definition":"Post-sampling status","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B69" t="str">
+        <f t="shared" si="14"/>
+        <v>{"column":"diseaseDetected","group":"diseaseSampling","uri":"urn:diseaseDetected","dataType":"String","definition":"Result of disease testing: True=Positive, False=Negative, No Confidence=Ambiguous","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B70" t="str">
+        <f t="shared" si="14"/>
+        <v>{"column":"fatal","group":"diseaseSampling","uri":"urn:fatal","dataType":"String","definition":"At time of sampling, presumed cause of death to be diseaseTested, mark [FALSE] if unknown","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B71" t="str">
+        <f t="shared" si="14"/>
+        <v>{"column":"testMethod","group":"diseaseSampling","uri":"urn:testMethod","dataType":"String","definition":"traditional PCR, quantitive PCR, realtime PCR, histology, Other","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B72" t="str">
+        <f t="shared" si="14"/>
+        <v>{"column":"quantityDected","group":"diseaseSampling","uri":"urn:quantityDected","dataType":"String","definition":"Number of zoospore detected. Needed to calculate Zoospore Equivalent Score (ZEscore), a measure of infection intensity (see Vredenburg et al 2010 doi: 10.1073/pnas.0914111107)","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B73" t="str">
+        <f t="shared" si="14"/>
+        <v>{"column":"dilutionFactor","group":"diseaseSampling","uri":"urn:dilutionFactor","dataType":"String","definition":"The dilution factor is needed to calculate Zoospore Equivalent Score (ZEscore), a measure of infection intensity (see Vredenburg et al 2010 doi: 10.1073/pnas.0914111107)","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B74" t="str">
+        <f t="shared" si="14"/>
+        <v>{"column":"cycleTimeFirstDetection","group":"diseaseSampling","uri":"urn:cycleTimeFirstDetection","dataType":"String","definition":"Cycle number ("c(t)") at which the qPCR machine first detects a positive for chytrid ( a measure of the amount of Bd or Bsal present)","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B75" t="str">
+        <f t="shared" si="14"/>
+        <v>{"column":"diagnosticLab","group":"diseaseSampling","uri":"urn:diagnosticLab","dataType":"String","definition":"Record the diagnostic lab if different than the diagnostic lab listed in the Project details or if more than one are used.","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B76" t="str">
+        <f t="shared" si="14"/>
+        <v>{"column":"zeScore","group":"diseaseSampling","uri":"urn:zeScore","dataType":"String","definition":"If present, these values may be entered (otherwise it will be calculated from the quantityDetected and dilutionFactor).","internal": false, "allowUnknown": false, "allowTBD": false}</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F45">
-    <sortCondition ref="C2:C45"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I47">
+    <sortCondition ref="G2:G47"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
setting up dataset revision folder in revised_data folder
</commit_message>
<xml_diff>
--- a/amphibianDisease/amphibianDisease.xlsx
+++ b/amphibianDisease/amphibianDisease.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdeck/IdeaProjects/geome-configurations/amphibianDisease/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68AFE70-0298-4649-AE1A-E8059D6EB867}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A08315E-CA17-6B44-BEF0-3B2AA9B96E69}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="460" windowWidth="13840" windowHeight="17540" xr2:uid="{EE213A37-7B2B-0548-A624-8FB513D29C9B}"/>
+    <workbookView xWindow="4040" yWindow="26140" windowWidth="13840" windowHeight="17540" xr2:uid="{EE213A37-7B2B-0548-A624-8FB513D29C9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="96">
   <si>
     <t>sampleID</t>
   </si>
@@ -294,16 +294,7 @@
     <t>testMethod</t>
   </si>
   <si>
-    <t>diseaseSampling</t>
-  </si>
-  <si>
     <t>zeScore</t>
-  </si>
-  <si>
-    <t>column</t>
-  </si>
-  <si>
-    <t>group</t>
   </si>
   <si>
     <t>uri</t>
@@ -713,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9974B0-4F07-3F40-862F-7C3240289FB3}">
   <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -754,6 +745,10 @@
       <c r="B2" t="s">
         <v>22</v>
       </c>
+      <c r="C2" t="str">
+        <f>_xlfn.CONCAT(A2," as ",B2, ",")</f>
+        <v>dateCollected as yearCollected|monthCollected|dayCollected,</v>
+      </c>
       <c r="G2" t="s">
         <v>73</v>
       </c>
@@ -765,6 +760,10 @@
       <c r="B3" t="s">
         <v>23</v>
       </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C45" si="0">_xlfn.CONCAT(A3," as ",B3, ",")</f>
+        <v>decimalLatitude as decimalLatitude,</v>
+      </c>
       <c r="G3" t="s">
         <v>73</v>
       </c>
@@ -776,6 +775,10 @@
       <c r="B4" t="s">
         <v>24</v>
       </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>decimalLongitude as decimalLongitude,</v>
+      </c>
       <c r="G4" t="s">
         <v>73</v>
       </c>
@@ -787,6 +790,10 @@
       <c r="B5" t="s">
         <v>38</v>
       </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>datum as horizontalDatum,</v>
+      </c>
       <c r="G5" t="s">
         <v>73</v>
       </c>
@@ -798,6 +805,10 @@
       <c r="B6" t="s">
         <v>39</v>
       </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>georeferenceSource as georeferenceProtocal,</v>
+      </c>
       <c r="G6" t="s">
         <v>73</v>
       </c>
@@ -809,6 +820,10 @@
       <c r="B7" t="s">
         <v>40</v>
       </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>elevation as minimumElevationInMeters|maximumElevationInMeters,</v>
+      </c>
       <c r="G7" t="s">
         <v>73</v>
       </c>
@@ -820,6 +835,10 @@
       <c r="B8" t="s">
         <v>28</v>
       </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>coordinateUncertaintyInMeters as coordinateUncertaintyInMeters,</v>
+      </c>
       <c r="G8" t="s">
         <v>73</v>
       </c>
@@ -831,6 +850,10 @@
       <c r="B9" t="s">
         <v>41</v>
       </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>depth as minimumDepthInMeters|maximumDepthInMeters,</v>
+      </c>
       <c r="G9" t="s">
         <v>73</v>
       </c>
@@ -842,6 +865,10 @@
       <c r="B10" t="s">
         <v>42</v>
       </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>Collector as collectorList,</v>
+      </c>
       <c r="G10" t="s">
         <v>73</v>
       </c>
@@ -853,6 +880,10 @@
       <c r="B11" t="s">
         <v>83</v>
       </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>ContactName as principalInvestigator,</v>
+      </c>
       <c r="G11" t="s">
         <v>73</v>
       </c>
@@ -864,6 +895,10 @@
       <c r="B12" t="s">
         <v>42</v>
       </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>Collector2 as collectorList,</v>
+      </c>
       <c r="G12" t="s">
         <v>73</v>
       </c>
@@ -875,6 +910,10 @@
       <c r="B13" t="s">
         <v>42</v>
       </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>Collector3 as collectorList,</v>
+      </c>
       <c r="G13" t="s">
         <v>73</v>
       </c>
@@ -886,6 +925,10 @@
       <c r="B14" t="s">
         <v>43</v>
       </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>verbatimLocality as locality,</v>
+      </c>
       <c r="G14" t="s">
         <v>73</v>
       </c>
@@ -897,6 +940,10 @@
       <c r="B15" t="s">
         <v>44</v>
       </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>Habitat as habitat,</v>
+      </c>
       <c r="G15" t="s">
         <v>73</v>
       </c>
@@ -908,6 +955,10 @@
       <c r="B16" t="s">
         <v>37</v>
       </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>eventRemarks as eventRemarks,</v>
+      </c>
       <c r="G16" t="s">
         <v>73</v>
       </c>
@@ -919,6 +970,10 @@
       <c r="B17" t="s">
         <v>52</v>
       </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>state_province as stateProvince,</v>
+      </c>
       <c r="G17" t="s">
         <v>73</v>
       </c>
@@ -930,6 +985,10 @@
       <c r="B18" t="s">
         <v>2</v>
       </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>sampleID as materialSampleID,</v>
+      </c>
       <c r="G18" t="s">
         <v>72</v>
       </c>
@@ -938,6 +997,10 @@
       <c r="A19" t="s">
         <v>1</v>
       </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>basisOfRecord as ,</v>
+      </c>
       <c r="G19" t="s">
         <v>72</v>
       </c>
@@ -952,6 +1015,10 @@
       <c r="B20" t="s">
         <v>3</v>
       </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>occurrenceID as occurrenceID,</v>
+      </c>
       <c r="G20" t="s">
         <v>72</v>
       </c>
@@ -963,6 +1030,10 @@
       <c r="B21" t="s">
         <v>4</v>
       </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>institutionCode as institutionCode,</v>
+      </c>
       <c r="G21" t="s">
         <v>72</v>
       </c>
@@ -974,6 +1045,10 @@
       <c r="B22" t="s">
         <v>5</v>
       </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>collectionCode as collectionCode,</v>
+      </c>
       <c r="G22" t="s">
         <v>72</v>
       </c>
@@ -985,6 +1060,10 @@
       <c r="B23" t="s">
         <v>6</v>
       </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>catalogNumber as catalogNumber,</v>
+      </c>
       <c r="G23" t="s">
         <v>72</v>
       </c>
@@ -996,6 +1075,10 @@
       <c r="B24" t="s">
         <v>66</v>
       </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>labNumber as otherCatalogNumbers,</v>
+      </c>
       <c r="F24" s="1" t="s">
         <v>65</v>
       </c>
@@ -1010,6 +1093,10 @@
       <c r="B25" t="s">
         <v>16</v>
       </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>genus as genus,</v>
+      </c>
       <c r="G25" t="s">
         <v>72</v>
       </c>
@@ -1021,6 +1108,10 @@
       <c r="B26" t="s">
         <v>17</v>
       </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>specificEpithet as specificEpithet,</v>
+      </c>
       <c r="G26" t="s">
         <v>72</v>
       </c>
@@ -1032,6 +1123,10 @@
       <c r="B27" t="s">
         <v>18</v>
       </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>infraspecificEpithet as infraspecificEpithet,</v>
+      </c>
       <c r="G27" t="s">
         <v>72</v>
       </c>
@@ -1043,6 +1138,10 @@
       <c r="B28" t="s">
         <v>19</v>
       </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>lifestage as lifestage,</v>
+      </c>
       <c r="G28" t="s">
         <v>72</v>
       </c>
@@ -1054,7 +1153,10 @@
       <c r="B29" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="5"/>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>fieldNumber as fieldNumber,</v>
+      </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="G29" t="s">
@@ -1068,6 +1170,10 @@
       <c r="B30" t="s">
         <v>56</v>
       </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>originalsource as establishmentMeans,</v>
+      </c>
       <c r="G30" t="s">
         <v>72</v>
       </c>
@@ -1082,28 +1188,26 @@
       <c r="B31" t="s">
         <v>20</v>
       </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>sex as sex,</v>
+      </c>
       <c r="G31" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
+      <c r="D32" t="s">
+        <v>88</v>
+      </c>
+      <c r="E32" t="s">
         <v>89</v>
-      </c>
-      <c r="C32" t="s">
-        <v>90</v>
-      </c>
-      <c r="D32" t="s">
-        <v>91</v>
-      </c>
-      <c r="E32" t="s">
-        <v>92</v>
       </c>
       <c r="F32" t="s">
         <v>75</v>
       </c>
       <c r="H32" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.25">
@@ -1113,18 +1217,19 @@
       <c r="B33" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>87</v>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>sampleType as sampleType,</v>
       </c>
       <c r="D33" s="3" t="str">
         <f>_xlfn.CONCAT("urn:",B33)</f>
         <v>urn:sampleType</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H33" t="s">
         <v>61</v>
@@ -1137,15 +1242,16 @@
       <c r="B34" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>87</v>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>diseaseLineage as diseaseLineage,</v>
       </c>
       <c r="D34" s="3" t="str">
         <f>_xlfn.CONCAT("urn:",B34)</f>
         <v>urn:diseaseLineage</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>64</v>
@@ -1158,15 +1264,16 @@
       <c r="B35" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>87</v>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>genotypeMethod as genotypeMethod,</v>
       </c>
       <c r="D35" s="3" t="str">
-        <f t="shared" ref="D35:D45" si="0">_xlfn.CONCAT("urn:",B35)</f>
+        <f t="shared" ref="D35:D45" si="1">_xlfn.CONCAT("urn:",B35)</f>
         <v>urn:genotypeMethod</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>67</v>
@@ -1179,15 +1286,16 @@
       <c r="B36" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>87</v>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>diseaseTested as diseaseTested,</v>
       </c>
       <c r="D36" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>urn:diseaseTested</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>76</v>
@@ -1203,18 +1311,19 @@
       <c r="B37" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>87</v>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>specimenDisposition as specimenDisposition,</v>
       </c>
       <c r="D37" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>urn:specimenDisposition</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H37" t="s">
         <v>57</v>
@@ -1227,15 +1336,16 @@
       <c r="B38" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>87</v>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>diseasedetected as diseaseDetected,</v>
       </c>
       <c r="D38" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>urn:diseaseDetected</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>77</v>
@@ -1251,15 +1361,16 @@
       <c r="B39" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>87</v>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal as fatal,</v>
       </c>
       <c r="D39" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>urn:fatal</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>68</v>
@@ -1275,15 +1386,16 @@
       <c r="B40" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>87</v>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>Test_Method as testMethod,</v>
       </c>
       <c r="D40" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>urn:testMethod</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F40" t="s">
         <v>60</v>
@@ -1296,15 +1408,16 @@
       <c r="B41" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>87</v>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>quantityDetected as quantityDected,</v>
       </c>
       <c r="D41" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>urn:quantityDected</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>78</v>
@@ -1317,18 +1430,19 @@
       <c r="B42" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>87</v>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>dilutionFactor as dilutionFactor,</v>
       </c>
       <c r="D42" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>urn:dilutionFactor</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.25">
@@ -1338,15 +1452,16 @@
       <c r="B43" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>87</v>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>cycleTimeFirstDetection as cycleTimeFirstDetection,</v>
       </c>
       <c r="D43" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>urn:cycleTimeFirstDetection</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>79</v>
@@ -1359,15 +1474,16 @@
       <c r="B44" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>87</v>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>diagnosticLab as diagnosticLab,</v>
       </c>
       <c r="D44" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>urn:diagnosticLab</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>80</v>
@@ -1378,17 +1494,18 @@
         <v>50</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C45" s="3" t="s">
         <v>87</v>
       </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>ZEscore as zeScore,</v>
+      </c>
       <c r="D45" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>urn:zeScore</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>81</v>
@@ -1419,370 +1536,370 @@
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B50" t="str">
         <f>_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B33,CHAR(34))</f>
-        <v>"column":"sampleType"</v>
+        <v>"":"sampleType"</v>
       </c>
       <c r="C50" t="str">
-        <f t="shared" ref="C50:F50" si="1">_xlfn.CONCAT(CHAR(34),C$32,CHAR(34),":",CHAR(34),C33,CHAR(34))</f>
-        <v>"group":"diseaseSampling"</v>
+        <f t="shared" ref="C50:F50" si="2">_xlfn.CONCAT(CHAR(34),C$32,CHAR(34),":",CHAR(34),C33,CHAR(34))</f>
+        <v>"":"sampleType as sampleType,"</v>
       </c>
       <c r="D50" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>"uri":"urn:sampleType"</v>
       </c>
       <c r="E50" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>"dataType":"String"</v>
       </c>
       <c r="F50" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>"definition":"Type of sample tested: eg, swabbing, blood, skin, liver"</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B51" t="str">
-        <f t="shared" ref="B51:F51" si="2">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B34,CHAR(34))</f>
-        <v>"column":"diseaseLineage"</v>
+        <f t="shared" ref="B51:F51" si="3">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B34,CHAR(34))</f>
+        <v>"":"diseaseLineage"</v>
       </c>
       <c r="C51" t="str">
-        <f t="shared" si="2"/>
-        <v>"group":"diseaseSampling"</v>
+        <f t="shared" si="3"/>
+        <v>"":"diseaseLineage as diseaseLineage,"</v>
       </c>
       <c r="D51" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"uri":"urn:diseaseLineage"</v>
       </c>
       <c r="E51" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"dataType":"String"</v>
       </c>
       <c r="F51" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"definition":"Specific genetic lineage detected (if available) NCBI URI (e.g., http://www.ncbi.nlm.nih.gov/biosample/xxxxxxx"</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B52" t="str">
-        <f t="shared" ref="B52:F52" si="3">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B35,CHAR(34))</f>
-        <v>"column":"genotypeMethod"</v>
+        <f t="shared" ref="B52:F52" si="4">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B35,CHAR(34))</f>
+        <v>"":"genotypeMethod"</v>
       </c>
       <c r="C52" t="str">
-        <f t="shared" si="3"/>
-        <v>"group":"diseaseSampling"</v>
+        <f t="shared" si="4"/>
+        <v>"":"genotypeMethod as genotypeMethod,"</v>
       </c>
       <c r="D52" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>"uri":"urn:genotypeMethod"</v>
       </c>
       <c r="E52" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>"dataType":"String"</v>
       </c>
       <c r="F52" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>"definition":"Genotyping methods used to determine diseaseLineage if present (e.g., whole genome sequencing, ITS sequencing, multilocus nuclear sequencing)."</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B53" t="str">
-        <f t="shared" ref="B53:F53" si="4">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B36,CHAR(34))</f>
-        <v>"column":"diseaseTested"</v>
+        <f t="shared" ref="B53:F53" si="5">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B36,CHAR(34))</f>
+        <v>"":"diseaseTested"</v>
       </c>
       <c r="C53" t="str">
-        <f t="shared" si="4"/>
-        <v>"group":"diseaseSampling"</v>
+        <f t="shared" si="5"/>
+        <v>"":"diseaseTested as diseaseTested,"</v>
       </c>
       <c r="D53" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>"uri":"urn:diseaseTested"</v>
       </c>
       <c r="E53" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>"dataType":"String"</v>
       </c>
       <c r="F53" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>"definition":"Controlled vocabulary: Bd, Bsal, Bd+Bsal, Other"</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B54" t="str">
-        <f t="shared" ref="B54:F54" si="5">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B37,CHAR(34))</f>
-        <v>"column":"specimenDisposition"</v>
+        <f t="shared" ref="B54:F54" si="6">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B37,CHAR(34))</f>
+        <v>"":"specimenDisposition"</v>
       </c>
       <c r="C54" t="str">
-        <f t="shared" si="5"/>
-        <v>"group":"diseaseSampling"</v>
+        <f t="shared" si="6"/>
+        <v>"":"specimenDisposition as specimenDisposition,"</v>
       </c>
       <c r="D54" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>"uri":"urn:specimenDisposition"</v>
       </c>
       <c r="E54" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>"dataType":"String"</v>
       </c>
       <c r="F54" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>"definition":"Post-sampling status"</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B55" t="str">
-        <f t="shared" ref="B55:F55" si="6">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B38,CHAR(34))</f>
-        <v>"column":"diseaseDetected"</v>
+        <f t="shared" ref="B55:F55" si="7">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B38,CHAR(34))</f>
+        <v>"":"diseaseDetected"</v>
       </c>
       <c r="C55" t="str">
-        <f t="shared" si="6"/>
-        <v>"group":"diseaseSampling"</v>
+        <f t="shared" si="7"/>
+        <v>"":"diseasedetected as diseaseDetected,"</v>
       </c>
       <c r="D55" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>"uri":"urn:diseaseDetected"</v>
       </c>
       <c r="E55" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>"dataType":"String"</v>
       </c>
       <c r="F55" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>"definition":"Result of disease testing: True=Positive, False=Negative, No Confidence=Ambiguous"</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B56" t="str">
-        <f t="shared" ref="B56:F56" si="7">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B39,CHAR(34))</f>
-        <v>"column":"fatal"</v>
+        <f t="shared" ref="B56:F56" si="8">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B39,CHAR(34))</f>
+        <v>"":"fatal"</v>
       </c>
       <c r="C56" t="str">
-        <f t="shared" si="7"/>
-        <v>"group":"diseaseSampling"</v>
+        <f t="shared" si="8"/>
+        <v>"":"fatal as fatal,"</v>
       </c>
       <c r="D56" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>"uri":"urn:fatal"</v>
       </c>
       <c r="E56" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>"dataType":"String"</v>
       </c>
       <c r="F56" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>"definition":"At time of sampling, presumed cause of death to be diseaseTested, mark [FALSE] if unknown"</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B57" t="str">
-        <f t="shared" ref="B57:F57" si="8">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B40,CHAR(34))</f>
-        <v>"column":"testMethod"</v>
+        <f t="shared" ref="B57:F57" si="9">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B40,CHAR(34))</f>
+        <v>"":"testMethod"</v>
       </c>
       <c r="C57" t="str">
-        <f t="shared" si="8"/>
-        <v>"group":"diseaseSampling"</v>
+        <f t="shared" si="9"/>
+        <v>"":"Test_Method as testMethod,"</v>
       </c>
       <c r="D57" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>"uri":"urn:testMethod"</v>
       </c>
       <c r="E57" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>"dataType":"String"</v>
       </c>
       <c r="F57" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>"definition":"traditional PCR, quantitive PCR, realtime PCR, histology, Other"</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B58" t="str">
-        <f t="shared" ref="B58:F58" si="9">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B41,CHAR(34))</f>
-        <v>"column":"quantityDected"</v>
+        <f t="shared" ref="B58:F58" si="10">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B41,CHAR(34))</f>
+        <v>"":"quantityDected"</v>
       </c>
       <c r="C58" t="str">
-        <f t="shared" si="9"/>
-        <v>"group":"diseaseSampling"</v>
+        <f t="shared" si="10"/>
+        <v>"":"quantityDetected as quantityDected,"</v>
       </c>
       <c r="D58" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>"uri":"urn:quantityDected"</v>
       </c>
       <c r="E58" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>"dataType":"String"</v>
       </c>
       <c r="F58" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>"definition":"Number of zoospore detected. Needed to calculate Zoospore Equivalent Score (ZEscore), a measure of infection intensity (see Vredenburg et al 2010 doi: 10.1073/pnas.0914111107)"</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B59" t="str">
-        <f t="shared" ref="B59:F59" si="10">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B42,CHAR(34))</f>
-        <v>"column":"dilutionFactor"</v>
+        <f t="shared" ref="B59:F59" si="11">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B42,CHAR(34))</f>
+        <v>"":"dilutionFactor"</v>
       </c>
       <c r="C59" t="str">
-        <f t="shared" si="10"/>
-        <v>"group":"diseaseSampling"</v>
+        <f t="shared" si="11"/>
+        <v>"":"dilutionFactor as dilutionFactor,"</v>
       </c>
       <c r="D59" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>"uri":"urn:dilutionFactor"</v>
       </c>
       <c r="E59" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>"dataType":"String"</v>
       </c>
       <c r="F59" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>"definition":"The dilution factor is needed to calculate Zoospore Equivalent Score (ZEscore), a measure of infection intensity (see Vredenburg et al 2010 doi: 10.1073/pnas.0914111107)"</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B60" t="str">
-        <f t="shared" ref="B60:F60" si="11">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B43,CHAR(34))</f>
-        <v>"column":"cycleTimeFirstDetection"</v>
+        <f t="shared" ref="B60:F60" si="12">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B43,CHAR(34))</f>
+        <v>"":"cycleTimeFirstDetection"</v>
       </c>
       <c r="C60" t="str">
-        <f t="shared" si="11"/>
-        <v>"group":"diseaseSampling"</v>
+        <f t="shared" si="12"/>
+        <v>"":"cycleTimeFirstDetection as cycleTimeFirstDetection,"</v>
       </c>
       <c r="D60" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>"uri":"urn:cycleTimeFirstDetection"</v>
       </c>
       <c r="E60" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>"dataType":"String"</v>
       </c>
       <c r="F60" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>"definition":"Cycle number ("c(t)") at which the qPCR machine first detects a positive for chytrid ( a measure of the amount of Bd or Bsal present)"</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B61" t="str">
-        <f t="shared" ref="B61:F61" si="12">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B44,CHAR(34))</f>
-        <v>"column":"diagnosticLab"</v>
+        <f t="shared" ref="B61:F61" si="13">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B44,CHAR(34))</f>
+        <v>"":"diagnosticLab"</v>
       </c>
       <c r="C61" t="str">
-        <f t="shared" si="12"/>
-        <v>"group":"diseaseSampling"</v>
+        <f t="shared" si="13"/>
+        <v>"":"diagnosticLab as diagnosticLab,"</v>
       </c>
       <c r="D61" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>"uri":"urn:diagnosticLab"</v>
       </c>
       <c r="E61" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>"dataType":"String"</v>
       </c>
       <c r="F61" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>"definition":"Record the diagnostic lab if different than the diagnostic lab listed in the Project details or if more than one are used."</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B62" t="str">
-        <f t="shared" ref="B62:F62" si="13">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B45,CHAR(34))</f>
-        <v>"column":"zeScore"</v>
+        <f t="shared" ref="B62:F62" si="14">_xlfn.CONCAT(CHAR(34),B$32,CHAR(34),":",CHAR(34),B45,CHAR(34))</f>
+        <v>"":"zeScore"</v>
       </c>
       <c r="C62" t="str">
-        <f t="shared" si="13"/>
-        <v>"group":"diseaseSampling"</v>
+        <f t="shared" si="14"/>
+        <v>"":"ZEscore as zeScore,"</v>
       </c>
       <c r="D62" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>"uri":"urn:zeScore"</v>
       </c>
       <c r="E62" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>"dataType":"String"</v>
       </c>
       <c r="F62" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>"definition":"If present, these values may be entered (otherwise it will be calculated from the quantityDetected and dilutionFactor)."</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B64" t="str">
         <f>_xlfn.CONCAT("{",B50,",",C50,",",D50,",",E50,",",F50,",",$A$63,"}")</f>
-        <v>{"column":"sampleType","group":"diseaseSampling","uri":"urn:sampleType","dataType":"String","definition":"Type of sample tested: eg, swabbing, blood, skin, liver","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+        <v>{"":"sampleType","":"sampleType as sampleType,","uri":"urn:sampleType","dataType":"String","definition":"Type of sample tested: eg, swabbing, blood, skin, liver","internal": false, "allowUnknown": false, "allowTBD": false}</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B65" t="str">
-        <f t="shared" ref="B65:B76" si="14">_xlfn.CONCAT("{",B51,",",C51,",",D51,",",E51,",",F51,",",$A$63,"}")</f>
-        <v>{"column":"diseaseLineage","group":"diseaseSampling","uri":"urn:diseaseLineage","dataType":"String","definition":"Specific genetic lineage detected (if available) NCBI URI (e.g., http://www.ncbi.nlm.nih.gov/biosample/xxxxxxx","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+        <f t="shared" ref="B65:B76" si="15">_xlfn.CONCAT("{",B51,",",C51,",",D51,",",E51,",",F51,",",$A$63,"}")</f>
+        <v>{"":"diseaseLineage","":"diseaseLineage as diseaseLineage,","uri":"urn:diseaseLineage","dataType":"String","definition":"Specific genetic lineage detected (if available) NCBI URI (e.g., http://www.ncbi.nlm.nih.gov/biosample/xxxxxxx","internal": false, "allowUnknown": false, "allowTBD": false}</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B66" t="str">
-        <f t="shared" si="14"/>
-        <v>{"column":"genotypeMethod","group":"diseaseSampling","uri":"urn:genotypeMethod","dataType":"String","definition":"Genotyping methods used to determine diseaseLineage if present (e.g., whole genome sequencing, ITS sequencing, multilocus nuclear sequencing).","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+        <f t="shared" si="15"/>
+        <v>{"":"genotypeMethod","":"genotypeMethod as genotypeMethod,","uri":"urn:genotypeMethod","dataType":"String","definition":"Genotyping methods used to determine diseaseLineage if present (e.g., whole genome sequencing, ITS sequencing, multilocus nuclear sequencing).","internal": false, "allowUnknown": false, "allowTBD": false}</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B67" t="str">
-        <f t="shared" si="14"/>
-        <v>{"column":"diseaseTested","group":"diseaseSampling","uri":"urn:diseaseTested","dataType":"String","definition":"Controlled vocabulary: Bd, Bsal, Bd+Bsal, Other","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+        <f t="shared" si="15"/>
+        <v>{"":"diseaseTested","":"diseaseTested as diseaseTested,","uri":"urn:diseaseTested","dataType":"String","definition":"Controlled vocabulary: Bd, Bsal, Bd+Bsal, Other","internal": false, "allowUnknown": false, "allowTBD": false}</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B68" t="str">
-        <f t="shared" si="14"/>
-        <v>{"column":"specimenDisposition","group":"diseaseSampling","uri":"urn:specimenDisposition","dataType":"String","definition":"Post-sampling status","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+        <f t="shared" si="15"/>
+        <v>{"":"specimenDisposition","":"specimenDisposition as specimenDisposition,","uri":"urn:specimenDisposition","dataType":"String","definition":"Post-sampling status","internal": false, "allowUnknown": false, "allowTBD": false}</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B69" t="str">
-        <f t="shared" si="14"/>
-        <v>{"column":"diseaseDetected","group":"diseaseSampling","uri":"urn:diseaseDetected","dataType":"String","definition":"Result of disease testing: True=Positive, False=Negative, No Confidence=Ambiguous","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+        <f t="shared" si="15"/>
+        <v>{"":"diseaseDetected","":"diseasedetected as diseaseDetected,","uri":"urn:diseaseDetected","dataType":"String","definition":"Result of disease testing: True=Positive, False=Negative, No Confidence=Ambiguous","internal": false, "allowUnknown": false, "allowTBD": false}</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B70" t="str">
-        <f t="shared" si="14"/>
-        <v>{"column":"fatal","group":"diseaseSampling","uri":"urn:fatal","dataType":"String","definition":"At time of sampling, presumed cause of death to be diseaseTested, mark [FALSE] if unknown","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+        <f t="shared" si="15"/>
+        <v>{"":"fatal","":"fatal as fatal,","uri":"urn:fatal","dataType":"String","definition":"At time of sampling, presumed cause of death to be diseaseTested, mark [FALSE] if unknown","internal": false, "allowUnknown": false, "allowTBD": false}</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B71" t="str">
-        <f t="shared" si="14"/>
-        <v>{"column":"testMethod","group":"diseaseSampling","uri":"urn:testMethod","dataType":"String","definition":"traditional PCR, quantitive PCR, realtime PCR, histology, Other","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+        <f t="shared" si="15"/>
+        <v>{"":"testMethod","":"Test_Method as testMethod,","uri":"urn:testMethod","dataType":"String","definition":"traditional PCR, quantitive PCR, realtime PCR, histology, Other","internal": false, "allowUnknown": false, "allowTBD": false}</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B72" t="str">
-        <f t="shared" si="14"/>
-        <v>{"column":"quantityDected","group":"diseaseSampling","uri":"urn:quantityDected","dataType":"String","definition":"Number of zoospore detected. Needed to calculate Zoospore Equivalent Score (ZEscore), a measure of infection intensity (see Vredenburg et al 2010 doi: 10.1073/pnas.0914111107)","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+        <f t="shared" si="15"/>
+        <v>{"":"quantityDected","":"quantityDetected as quantityDected,","uri":"urn:quantityDected","dataType":"String","definition":"Number of zoospore detected. Needed to calculate Zoospore Equivalent Score (ZEscore), a measure of infection intensity (see Vredenburg et al 2010 doi: 10.1073/pnas.0914111107)","internal": false, "allowUnknown": false, "allowTBD": false}</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B73" t="str">
-        <f t="shared" si="14"/>
-        <v>{"column":"dilutionFactor","group":"diseaseSampling","uri":"urn:dilutionFactor","dataType":"String","definition":"The dilution factor is needed to calculate Zoospore Equivalent Score (ZEscore), a measure of infection intensity (see Vredenburg et al 2010 doi: 10.1073/pnas.0914111107)","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+        <f t="shared" si="15"/>
+        <v>{"":"dilutionFactor","":"dilutionFactor as dilutionFactor,","uri":"urn:dilutionFactor","dataType":"String","definition":"The dilution factor is needed to calculate Zoospore Equivalent Score (ZEscore), a measure of infection intensity (see Vredenburg et al 2010 doi: 10.1073/pnas.0914111107)","internal": false, "allowUnknown": false, "allowTBD": false}</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B74" t="str">
-        <f t="shared" si="14"/>
-        <v>{"column":"cycleTimeFirstDetection","group":"diseaseSampling","uri":"urn:cycleTimeFirstDetection","dataType":"String","definition":"Cycle number ("c(t)") at which the qPCR machine first detects a positive for chytrid ( a measure of the amount of Bd or Bsal present)","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+        <f t="shared" si="15"/>
+        <v>{"":"cycleTimeFirstDetection","":"cycleTimeFirstDetection as cycleTimeFirstDetection,","uri":"urn:cycleTimeFirstDetection","dataType":"String","definition":"Cycle number ("c(t)") at which the qPCR machine first detects a positive for chytrid ( a measure of the amount of Bd or Bsal present)","internal": false, "allowUnknown": false, "allowTBD": false}</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B75" t="str">
-        <f t="shared" si="14"/>
-        <v>{"column":"diagnosticLab","group":"diseaseSampling","uri":"urn:diagnosticLab","dataType":"String","definition":"Record the diagnostic lab if different than the diagnostic lab listed in the Project details or if more than one are used.","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+        <f t="shared" si="15"/>
+        <v>{"":"diagnosticLab","":"diagnosticLab as diagnosticLab,","uri":"urn:diagnosticLab","dataType":"String","definition":"Record the diagnostic lab if different than the diagnostic lab listed in the Project details or if more than one are used.","internal": false, "allowUnknown": false, "allowTBD": false}</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B76" t="str">
-        <f t="shared" si="14"/>
-        <v>{"column":"zeScore","group":"diseaseSampling","uri":"urn:zeScore","dataType":"String","definition":"If present, these values may be entered (otherwise it will be calculated from the quantityDetected and dilutionFactor).","internal": false, "allowUnknown": false, "allowTBD": false}</v>
+        <f t="shared" si="15"/>
+        <v>{"":"zeScore","":"ZEscore as zeScore,","uri":"urn:zeScore","dataType":"String","definition":"If present, these values may be entered (otherwise it will be calculated from the quantityDetected and dilutionFactor).","internal": false, "allowUnknown": false, "allowTBD": false}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>